<commit_message>
verbrauch ist 0 if value missing, addded display by verbrauch
verbrauch ist 0 if value missing, addded display by verbrauch
</commit_message>
<xml_diff>
--- a/preprocessed_df.xlsx
+++ b/preprocessed_df.xlsx
@@ -6142,7 +6142,9 @@
       </c>
       <c r="S13" t="inlineStr"/>
       <c r="T13" t="inlineStr"/>
-      <c r="U13" t="inlineStr"/>
+      <c r="U13" t="n">
+        <v>0</v>
+      </c>
       <c r="V13" t="n">
         <v>5</v>
       </c>
@@ -9319,7 +9321,9 @@
       </c>
       <c r="S20" t="inlineStr"/>
       <c r="T20" t="inlineStr"/>
-      <c r="U20" t="inlineStr"/>
+      <c r="U20" t="n">
+        <v>0</v>
+      </c>
       <c r="V20" t="n">
         <v>5</v>
       </c>
@@ -17830,7 +17834,9 @@
       <c r="R39" t="inlineStr"/>
       <c r="S39" t="inlineStr"/>
       <c r="T39" t="inlineStr"/>
-      <c r="U39" t="inlineStr"/>
+      <c r="U39" t="n">
+        <v>0</v>
+      </c>
       <c r="V39" t="inlineStr"/>
       <c r="W39" t="inlineStr"/>
       <c r="X39" t="inlineStr"/>
@@ -19636,7 +19642,9 @@
       </c>
       <c r="S43" t="inlineStr"/>
       <c r="T43" t="inlineStr"/>
-      <c r="U43" t="inlineStr"/>
+      <c r="U43" t="n">
+        <v>0</v>
+      </c>
       <c r="V43" t="n">
         <v>5</v>
       </c>
@@ -22336,7 +22344,9 @@
       </c>
       <c r="S49" t="inlineStr"/>
       <c r="T49" t="inlineStr"/>
-      <c r="U49" t="inlineStr"/>
+      <c r="U49" t="n">
+        <v>0</v>
+      </c>
       <c r="V49" t="n">
         <v>5</v>
       </c>
@@ -24545,7 +24555,9 @@
       <c r="R54" t="inlineStr"/>
       <c r="S54" t="inlineStr"/>
       <c r="T54" t="inlineStr"/>
-      <c r="U54" t="inlineStr"/>
+      <c r="U54" t="n">
+        <v>0</v>
+      </c>
       <c r="V54" t="inlineStr"/>
       <c r="W54" t="inlineStr"/>
       <c r="X54" t="inlineStr"/>
@@ -24954,7 +24966,9 @@
       <c r="R55" t="inlineStr"/>
       <c r="S55" t="inlineStr"/>
       <c r="T55" t="inlineStr"/>
-      <c r="U55" t="inlineStr"/>
+      <c r="U55" t="n">
+        <v>0</v>
+      </c>
       <c r="V55" t="inlineStr"/>
       <c r="W55" t="inlineStr"/>
       <c r="X55" t="inlineStr"/>
@@ -26249,7 +26263,9 @@
       <c r="R58" t="inlineStr"/>
       <c r="S58" t="inlineStr"/>
       <c r="T58" t="inlineStr"/>
-      <c r="U58" t="inlineStr"/>
+      <c r="U58" t="n">
+        <v>0</v>
+      </c>
       <c r="V58" t="inlineStr"/>
       <c r="W58" t="inlineStr"/>
       <c r="X58" t="inlineStr"/>
@@ -27103,7 +27119,9 @@
       <c r="R60" t="inlineStr"/>
       <c r="S60" t="inlineStr"/>
       <c r="T60" t="inlineStr"/>
-      <c r="U60" t="inlineStr"/>
+      <c r="U60" t="n">
+        <v>0</v>
+      </c>
       <c r="V60" t="inlineStr"/>
       <c r="W60" t="inlineStr"/>
       <c r="X60" t="inlineStr"/>

</xml_diff>